<commit_message>
Lots of js stuff. Got barcodes working great and registration overrides!
</commit_message>
<xml_diff>
--- a/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
+++ b/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
@@ -10,6 +10,7 @@
     <sheet name="model" sheetId="1" r:id="rId1"/>
     <sheet name="settings" sheetId="2" r:id="rId2"/>
     <sheet name="survey" sheetId="3" r:id="rId3"/>
+    <sheet name="properties" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>type</t>
   </si>
@@ -35,15 +36,6 @@
     <t>authorization_id</t>
   </si>
   <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>min_range</t>
-  </si>
-  <si>
-    <t>max_range</t>
-  </si>
-  <si>
     <t>authorization_name</t>
   </si>
   <si>
@@ -102,13 +94,52 @@
   </si>
   <si>
     <t>We are not giving volunteers the ability to create or edit authorizations. This table is here only for the implementation of overriding authorization rules</t>
+  </si>
+  <si>
+    <t>partition</t>
+  </si>
+  <si>
+    <t>aspect</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>security</t>
+  </si>
+  <si>
+    <t>unverifiedUserCanCreate</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>filterTypeOnCreation</t>
+  </si>
+  <si>
+    <t>READ_ONLY</t>
+  </si>
+  <si>
+    <t>locked</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>ranges</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,6 +171,13 @@
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -239,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -257,6 +295,13 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B7"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -618,18 +663,18 @@
     </row>
     <row r="3" spans="1:2" ht="23">
       <c r="A3" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="23">
       <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="23">
@@ -637,7 +682,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="23">
@@ -645,15 +690,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="23">
-      <c r="A7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -682,27 +719,27 @@
   <sheetData>
     <row r="1" spans="1:3" ht="23">
       <c r="A1" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23">
       <c r="A2" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="23">
       <c r="A3" s="10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" s="11">
         <v>20160824</v>
@@ -711,28 +748,28 @@
     </row>
     <row r="4" spans="1:3" ht="23">
       <c r="A4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3" ht="23">
       <c r="A5" s="10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="23">
       <c r="A6" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6" s="12"/>
     </row>
@@ -758,34 +795,122 @@
   <sheetData>
     <row r="1" spans="1:8" s="9" customFormat="1" ht="23">
       <c r="A1" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H1" s="16"/>
     </row>
     <row r="2" spans="1:8">
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
+      <c r="C1" s="17" t="s">
         <v>26</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit of just a bunch of changing whether things are strings or boolean and I'm not sure if I'm making the right choices, but I don't see how it could affect suitcase working. I also deleted the unnecessary tables
</commit_message>
<xml_diff>
--- a/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
+++ b/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>type</t>
   </si>
@@ -133,6 +133,27 @@
   </si>
   <si>
     <t>ranges</t>
+  </si>
+  <si>
+    <t>FormType</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>FormType.formType</t>
+  </si>
+  <si>
+    <t>SURVEY</t>
+  </si>
+  <si>
+    <t>SurveyUtil</t>
+  </si>
+  <si>
+    <t>SurveyUtil.formId</t>
+  </si>
+  <si>
+    <t>wrong_form</t>
   </si>
 </sst>
 </file>
@@ -635,7 +656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -837,10 +858,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -911,6 +932,40 @@
       </c>
       <c r="E4" s="19" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit on Wednesday. Not confirmed that everything is working. In particular item_description is not being recognized and it is breaking overrides
</commit_message>
<xml_diff>
--- a/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
+++ b/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
   <si>
     <t>type</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>wrong_form</t>
+  </si>
+  <si>
+    <t>item_description</t>
   </si>
 </sst>
 </file>
@@ -258,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -294,11 +297,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -323,6 +337,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -712,6 +728,14 @@
       </c>
       <c r="B6" s="6" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="23">
+      <c r="A7" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -860,7 +884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
A lot of changes from the weekend
</commit_message>
<xml_diff>
--- a/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
+++ b/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>type</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>string</t>
-  </si>
-  <si>
-    <t>authorization_id</t>
   </si>
   <si>
     <t>authorization_name</t>
@@ -163,7 +160,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -173,12 +170,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -312,33 +303,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -695,47 +684,39 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="23">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="23">
-      <c r="A3" s="5" t="s">
+    <row r="4" spans="1:2" ht="23">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="23">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="23">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="23">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="23">
+      <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="23">
-      <c r="A6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="23">
-      <c r="A7" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>44</v>
+      <c r="B6" s="19" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -763,60 +744,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="23">
+      <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="23">
-      <c r="A2" s="10" t="s">
+      <c r="B2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:3" ht="23">
+      <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B3" s="9">
+        <v>20160824</v>
+      </c>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:3" ht="23">
+      <c r="A4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" ht="23">
+      <c r="A5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="12"/>
-    </row>
-    <row r="3" spans="1:3" ht="23">
-      <c r="A3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="11">
-        <v>20160824</v>
-      </c>
-      <c r="C3" s="12"/>
-    </row>
-    <row r="4" spans="1:3" ht="23">
-      <c r="A4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="12"/>
-    </row>
-    <row r="5" spans="1:3" ht="23">
-      <c r="A5" s="10" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="23">
+      <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="23">
-      <c r="A6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="12"/>
+      <c r="B6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -838,36 +819,36 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" ht="23">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="23">
+      <c r="A1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8">
       <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
         <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -891,105 +872,105 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="C2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="D2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="D3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="17" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="17" t="s">
+      <c r="E5" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="17" t="s">
+      <c r="C6" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="17" t="s">
+      <c r="E6" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes from monday. Suitcase with UI still not working.
</commit_message>
<xml_diff>
--- a/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
+++ b/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>authorizations</t>
   </si>
   <si>
-    <t>Authorization</t>
-  </si>
-  <si>
     <t>clause</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>item_description</t>
+  </si>
+  <si>
+    <t>Authorizations</t>
   </si>
 </sst>
 </file>
@@ -661,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -684,7 +684,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="23">
@@ -716,7 +716,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -733,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -787,7 +787,7 @@
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="23">
@@ -821,34 +821,34 @@
   <sheetData>
     <row r="1" spans="1:8" s="7" customFormat="1" ht="23">
       <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>20</v>
       </c>
       <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8">
       <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
         <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -873,13 +873,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>25</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>0</v>
@@ -890,87 +890,87 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="C2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>29</v>
-      </c>
       <c r="E2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>27</v>
-      </c>
       <c r="C3" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>27</v>
-      </c>
       <c r="C4" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="C5" s="15" t="s">
         <v>37</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>38</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change config directory back to red cross demo, also edit forms to be compatable with rev 210 translations changes
</commit_message>
<xml_diff>
--- a/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
+++ b/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/redcross/app-designer/app/config/tables/authorizations/forms/authorizations/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -14,6 +19,9 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -78,9 +86,6 @@
     <t>values_list</t>
   </si>
   <si>
-    <t>display.text</t>
-  </si>
-  <si>
     <t>calculation</t>
   </si>
   <si>
@@ -163,6 +168,9 @@
   </si>
   <si>
     <t>is_simple</t>
+  </si>
+  <si>
+    <t>display.prompt.text</t>
   </si>
 </sst>
 </file>
@@ -367,6 +375,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -694,17 +707,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23">
+    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -712,15 +725,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="23">
+    <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="23">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -728,7 +741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23">
+    <row r="4" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -736,7 +749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23">
+    <row r="5" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -744,46 +757,41 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="23">
+    <row r="6" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="23">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="23">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="23">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -795,13 +803,13 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
     <col min="2" max="3" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23">
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -812,7 +820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="23">
+    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -821,7 +829,7 @@
       </c>
       <c r="C2" s="10"/>
     </row>
-    <row r="3" spans="1:3" ht="23">
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
@@ -830,7 +838,7 @@
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:3" ht="23">
+    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -839,16 +847,16 @@
       </c>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:3" ht="23">
+    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="23">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
@@ -859,11 +867,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -871,13 +874,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" ht="23">
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -894,28 +897,23 @@
         <v>1</v>
       </c>
       <c r="F1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="14"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -927,17 +925,17 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>24</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>0</v>
@@ -946,98 +944,93 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="C2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>28</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>29</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>31</v>
-      </c>
       <c r="D4" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="C5" s="15" t="s">
         <v>36</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>37</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="15" t="s">
+      <c r="B6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>39</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>40</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Text changes and query changes
</commit_message>
<xml_diff>
--- a/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
+++ b/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/redcross/app-designer/app/config/tables/authorizations/forms/authorizations/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="1180" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="3760" yWindow="1180" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -20,11 +15,11 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -195,13 +190,13 @@
     <t>choose_authorization</t>
   </si>
   <si>
-    <t>Choose an Authorization</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
     <t>defaultAccessOnCreation</t>
+  </si>
+  <si>
+    <t>Choose a Distribution</t>
   </si>
 </sst>
 </file>
@@ -742,13 +737,13 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -756,7 +751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="24">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -764,7 +759,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="24">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -772,7 +767,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="24">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -780,7 +775,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="24">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -788,7 +783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="24">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -796,7 +791,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="24">
       <c r="A7" s="18" t="s">
         <v>2</v>
       </c>
@@ -804,7 +799,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="24">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -812,7 +807,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="24">
       <c r="A9" s="18" t="s">
         <v>2</v>
       </c>
@@ -820,7 +815,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="24">
       <c r="A10" s="18" t="s">
         <v>2</v>
       </c>
@@ -828,7 +823,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="24">
       <c r="A11" s="18" t="s">
         <v>2</v>
       </c>
@@ -836,7 +831,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="24">
       <c r="A12" s="18" t="s">
         <v>2</v>
       </c>
@@ -847,6 +842,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -854,24 +854,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="3" max="3" width="45.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -879,16 +884,21 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -900,13 +910,13 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
     <col min="2" max="3" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="24">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -917,7 +927,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="24">
       <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
@@ -926,7 +936,7 @@
       </c>
       <c r="C2" s="10"/>
     </row>
-    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="24">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -935,7 +945,7 @@
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="24">
       <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
@@ -944,7 +954,7 @@
       </c>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="24">
       <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
@@ -953,7 +963,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="24">
       <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
@@ -964,6 +974,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -975,9 +990,9 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="24">
       <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
@@ -1001,7 +1016,7 @@
       </c>
       <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="C2" t="s">
         <v>18</v>
       </c>
@@ -1011,6 +1026,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1018,13 +1038,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="15" t="s">
         <v>20</v>
       </c>
@@ -1041,7 +1061,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
@@ -1058,7 +1078,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="15" t="s">
         <v>23</v>
       </c>
@@ -1066,7 +1086,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>2</v>
@@ -1075,7 +1095,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="15" t="s">
         <v>23</v>
       </c>
@@ -1092,7 +1112,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="15" t="s">
         <v>32</v>
       </c>
@@ -1109,7 +1129,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="15" t="s">
         <v>36</v>
       </c>
@@ -1129,5 +1149,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
move appGreece to app and zip up old /app into old_app.zip. Make schema changes to xlsx forms. No changes to any app level logic yet, but all xlsx files can be converted (except that custom_individual is making a warning message about type in relation to async assign).
</commit_message>
<xml_diff>
--- a/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
+++ b/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/new_redcross_repos/redcross-app-designer/appGreece/config/tables/authorizations/forms/authorizations/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="1180" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="7160" yWindow="5740" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -15,18 +20,18 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
   <si>
     <t>type</t>
   </si>
@@ -85,9 +90,6 @@
     <t>note</t>
   </si>
   <si>
-    <t>We are not giving volunteers the ability to create or edit authorizations. This table is here only for the implementation of overriding authorization rules</t>
-  </si>
-  <si>
     <t>partition</t>
   </si>
   <si>
@@ -121,9 +123,6 @@
     <t>true</t>
   </si>
   <si>
-    <t>ranges</t>
-  </si>
-  <si>
     <t>FormType</t>
   </si>
   <si>
@@ -145,18 +144,6 @@
     <t>wrong_form</t>
   </si>
   <si>
-    <t>item_description</t>
-  </si>
-  <si>
-    <t>assigned_code</t>
-  </si>
-  <si>
-    <t>is_active</t>
-  </si>
-  <si>
-    <t>is_simple</t>
-  </si>
-  <si>
     <t>display.prompt.text</t>
   </si>
   <si>
@@ -169,12 +156,6 @@
     <t>Authorizations</t>
   </si>
   <si>
-    <t>delivery_table</t>
-  </si>
-  <si>
-    <t>delivery_form</t>
-  </si>
-  <si>
     <t>string_token</t>
   </si>
   <si>
@@ -184,9 +165,6 @@
     <t>authorization_details</t>
   </si>
   <si>
-    <t>Authorization Details</t>
-  </si>
-  <si>
     <t>choose_authorization</t>
   </si>
   <si>
@@ -197,13 +175,76 @@
   </si>
   <si>
     <t>Choose a Distribution</t>
+  </si>
+  <si>
+    <t>Distribution Details</t>
+  </si>
+  <si>
+    <t>تفاصيل التوزيع</t>
+  </si>
+  <si>
+    <t>جزییات توزیع</t>
+  </si>
+  <si>
+    <t>Detalles de distribución</t>
+  </si>
+  <si>
+    <t>اختيار توزيعا</t>
+  </si>
+  <si>
+    <t>انتخاب توزیع</t>
+  </si>
+  <si>
+    <t>Elegir una distribución</t>
+  </si>
+  <si>
+    <t>text.arabic</t>
+  </si>
+  <si>
+    <t>text.farsi</t>
+  </si>
+  <si>
+    <t>Λεπτομέρειες διανομής</t>
+  </si>
+  <si>
+    <t>Επιλέξτε διανομή</t>
+  </si>
+  <si>
+    <t>text.greek</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>custom_delivery_form_id</t>
+  </si>
+  <si>
+    <t>item_pack_description</t>
+  </si>
+  <si>
+    <t>report_version</t>
+  </si>
+  <si>
+    <t>restrict_overrides</t>
+  </si>
+  <si>
+    <t>status_reason</t>
+  </si>
+  <si>
+    <t>summary_form_id</t>
+  </si>
+  <si>
+    <t>date_created</t>
+  </si>
+  <si>
+    <t>We are not giving volunteers the ability to create or edit authorizations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -252,6 +293,19 @@
       <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -311,7 +365,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -358,6 +412,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -366,7 +429,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -391,6 +454,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -731,19 +799,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24">
+    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -751,154 +819,193 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="24">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="24">
+    <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="24">
+      <c r="B4" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="24">
-      <c r="A6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="4" t="s">
+    <row r="7" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="24">
-      <c r="A7" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="24">
+    <row r="8" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="24">
-      <c r="A9" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="24">
-      <c r="A10" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="24">
-      <c r="A11" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="24">
+      <c r="B8" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>48</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="45.83203125" customWidth="1"/>
+    <col min="2" max="3" width="43" customWidth="1"/>
+    <col min="4" max="4" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E2" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -907,16 +1014,16 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
     <col min="2" max="3" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24">
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -924,10 +1031,10 @@
         <v>7</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="24">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
@@ -936,16 +1043,16 @@
       </c>
       <c r="C2" s="10"/>
     </row>
-    <row r="3" spans="1:3" ht="24">
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="9">
-        <v>20160824</v>
+        <v>20170919</v>
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:3" ht="24">
+    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
@@ -954,16 +1061,16 @@
       </c>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:3" ht="24">
+    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
@@ -974,11 +1081,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -987,12 +1089,12 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" ht="24">
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
@@ -1009,28 +1111,23 @@
         <v>1</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>17</v>
       </c>
       <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1038,21 +1135,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>22</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>0</v>
@@ -1061,98 +1158,93 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="C2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="17" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="17" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="15" t="s">
+      <c r="B5" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="D5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="15" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="15" t="s">
+      <c r="B6" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="15" t="s">
+      <c r="D6" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>36</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add back columns in entitlements and authorizations necessary for CTP use case
</commit_message>
<xml_diff>
--- a/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
+++ b/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/new_redcross_repos/redcross-app-designer/appGreece/config/tables/authorizations/forms/authorizations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/new_redcross_repos/redcross-app-designer/app/config/tables/authorizations/forms/authorizations/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7160" yWindow="5740" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="7160" yWindow="5740" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
   <si>
     <t>type</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>We are not giving volunteers the ability to create or edit authorizations</t>
+  </si>
+  <si>
+    <t>item_pack_ranges</t>
   </si>
 </sst>
 </file>
@@ -799,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -880,7 +883,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -888,23 +891,23 @@
         <v>2</v>
       </c>
       <c r="B10" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="23" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="22" t="s">
+    <row r="12" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="22" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -912,14 +915,22 @@
         <v>2</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1135,7 +1146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
handle the cleaning of additional custom form rows upon ignoring changes and exiting from a base custom row
</commit_message>
<xml_diff>
--- a/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
+++ b/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7160" yWindow="5740" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="15180" yWindow="9460" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
   <si>
     <t>type</t>
   </si>
@@ -42,9 +42,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>authorization_name</t>
-  </si>
-  <si>
     <t>item_pack_id</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>security</t>
   </si>
   <si>
-    <t>unverifiedUserCanCreate</t>
-  </si>
-  <si>
     <t>boolean</t>
   </si>
   <si>
@@ -117,24 +111,12 @@
     <t>locked</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
-    <t>FormType</t>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
-    <t>FormType.formType</t>
-  </si>
-  <si>
-    <t>SURVEY</t>
-  </si>
-  <si>
     <t>SurveyUtil</t>
   </si>
   <si>
@@ -241,6 +223,9 @@
   </si>
   <si>
     <t>item_pack_ranges</t>
+  </si>
+  <si>
+    <t>data('authorization_name)</t>
   </si>
 </sst>
 </file>
@@ -804,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -843,7 +828,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -851,7 +836,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -859,7 +844,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -867,7 +852,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -875,7 +860,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -883,7 +868,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -891,7 +876,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -899,7 +884,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -907,7 +892,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -915,7 +900,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -923,7 +908,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -931,7 +916,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -957,62 +942,62 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>49</v>
-      </c>
       <c r="E2" s="20" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>53</v>
-      </c>
       <c r="F3" s="20" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1024,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1036,27 +1021,27 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="9">
         <v>20170919</v>
@@ -1065,28 +1050,28 @@
     </row>
     <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="C6" s="10"/>
     </row>
@@ -1107,34 +1092,34 @@
   <sheetData>
     <row r="1" spans="1:8" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1144,114 +1129,80 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>23</v>
-      </c>
       <c r="C2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>24</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="C3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="17" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add missing for_individual field into authorizations table
</commit_message>
<xml_diff>
--- a/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
+++ b/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/new_redcross_repos/redcross-app-designer/app/config/tables/authorizations/forms/authorizations/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28540" windowHeight="18880" tabRatio="989" activeTab="1"/>
+    <workbookView xWindow="3000" yWindow="1880" windowWidth="28540" windowHeight="18880" tabRatio="989" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -18,13 +13,13 @@
     <sheet name="survey" sheetId="4" r:id="rId4"/>
     <sheet name="properties" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -34,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
   <si>
     <t>type</t>
   </si>
@@ -235,6 +230,12 @@
   </si>
   <si>
     <t>Date Created</t>
+  </si>
+  <si>
+    <t>for_individual</t>
+  </si>
+  <si>
+    <t>Generate Entitlement for Individual or Benefiiciary_Entity</t>
   </si>
 </sst>
 </file>
@@ -550,7 +551,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -585,7 +586,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -762,7 +763,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -770,15 +771,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,7 +787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="23">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -794,7 +795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="23">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -802,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="23">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -810,7 +811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="23">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -818,7 +819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="23">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -826,7 +827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="23">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -834,7 +835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="23">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -842,7 +843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="23">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -850,7 +851,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="23">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -858,7 +859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="23">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -866,7 +867,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="23">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -874,7 +875,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="23">
       <c r="A13" s="6" t="s">
         <v>2</v>
       </c>
@@ -882,7 +883,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="23">
       <c r="A14" s="6" t="s">
         <v>2</v>
       </c>
@@ -890,17 +891,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="23">
       <c r="A15" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="23">
+      <c r="A16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -908,11 +922,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="25.1640625" customWidth="1"/>
@@ -920,7 +934,7 @@
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -940,7 +954,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -952,7 +966,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="17">
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
@@ -964,7 +978,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -972,7 +986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
@@ -980,7 +994,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
@@ -988,7 +1002,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
@@ -996,7 +1010,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
@@ -1004,7 +1018,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
@@ -1012,7 +1026,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
@@ -1020,7 +1034,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
@@ -1028,7 +1042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -1036,7 +1050,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="12" t="s">
         <v>12</v>
       </c>
@@ -1044,7 +1058,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="12" t="s">
         <v>13</v>
       </c>
@@ -1052,7 +1066,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="12" t="s">
         <v>14</v>
       </c>
@@ -1060,12 +1074,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
+    <row r="16" spans="1:6">
+      <c r="A16" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1077,9 +1101,9 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="23">
       <c r="A1" s="14" t="s">
         <v>34</v>
       </c>
@@ -1090,7 +1114,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="23">
       <c r="A2" s="17" t="s">
         <v>37</v>
       </c>
@@ -1099,7 +1123,7 @@
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="23">
       <c r="A3" s="17" t="s">
         <v>39</v>
       </c>
@@ -1108,7 +1132,7 @@
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="23">
       <c r="A4" s="17" t="s">
         <v>40</v>
       </c>
@@ -1117,7 +1141,7 @@
       </c>
       <c r="C4" s="19"/>
     </row>
-    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="23">
       <c r="A5" s="17" t="s">
         <v>41</v>
       </c>
@@ -1126,7 +1150,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="23">
       <c r="A6" s="17" t="s">
         <v>43</v>
       </c>
@@ -1138,6 +1162,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1149,9 +1178,9 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8" s="16" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="16" customFormat="1" ht="23">
       <c r="A1" s="15" t="s">
         <v>45</v>
       </c>
@@ -1175,7 +1204,7 @@
       </c>
       <c r="H1" s="22"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="C2" t="s">
         <v>50</v>
       </c>
@@ -1186,6 +1215,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1193,13 +1227,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="23" t="s">
         <v>52</v>
       </c>
@@ -1216,7 +1250,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="23" t="s">
         <v>55</v>
       </c>
@@ -1233,7 +1267,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="23" t="s">
         <v>55</v>
       </c>
@@ -1250,7 +1284,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="23" t="s">
         <v>62</v>
       </c>
@@ -1270,5 +1304,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
for_member, member_id, custom_member_form_id, custom_member_row_id
</commit_message>
<xml_diff>
--- a/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
+++ b/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/new_redcross_repos/redcross-app-designer/app/config/tables/authorizations/forms/authorizations/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1880" windowWidth="28540" windowHeight="18880" tabRatio="989" activeTab="4"/>
+    <workbookView xWindow="3000" yWindow="1880" windowWidth="28540" windowHeight="18880" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -15,11 +20,11 @@
   </sheets>
   <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="70">
   <si>
     <t>type</t>
   </si>
@@ -236,6 +241,9 @@
   </si>
   <si>
     <t>Generate Entitlement for Individual or Benefiiciary_Entity</t>
+  </si>
+  <si>
+    <t>for_member</t>
   </si>
 </sst>
 </file>
@@ -763,7 +771,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -773,13 +781,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23">
+    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -787,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="23">
+    <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -795,7 +807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="23">
+    <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -803,7 +815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23">
+    <row r="4" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -811,7 +823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23">
+    <row r="5" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -819,7 +831,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="23">
+    <row r="6" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -827,7 +839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="23">
+    <row r="7" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -835,7 +847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23">
+    <row r="8" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -843,7 +855,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="23">
+    <row r="9" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -851,7 +863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="23">
+    <row r="10" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -859,7 +871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="23">
+    <row r="11" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -867,7 +879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="23">
+    <row r="12" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -875,7 +887,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="23">
+    <row r="13" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>2</v>
       </c>
@@ -883,7 +895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="23">
+    <row r="14" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>2</v>
       </c>
@@ -891,7 +903,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="23">
+    <row r="15" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>2</v>
       </c>
@@ -899,22 +911,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="23">
+    <row r="16" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -926,7 +933,7 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="25.1640625" customWidth="1"/>
@@ -934,7 +941,7 @@
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -954,7 +961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -966,7 +973,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" ht="17">
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
@@ -978,7 +985,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -986,7 +993,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
@@ -994,7 +1001,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
@@ -1002,7 +1009,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
@@ -1010,7 +1017,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
@@ -1018,7 +1025,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
@@ -1026,7 +1033,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
@@ -1034,7 +1041,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
@@ -1042,7 +1049,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -1050,7 +1057,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>12</v>
       </c>
@@ -1058,7 +1065,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>13</v>
       </c>
@@ -1066,7 +1073,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>14</v>
       </c>
@@ -1074,7 +1081,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>67</v>
       </c>
@@ -1085,11 +1092,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1101,9 +1103,9 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="23">
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>34</v>
       </c>
@@ -1114,7 +1116,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="23">
+    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>37</v>
       </c>
@@ -1123,7 +1125,7 @@
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" ht="23">
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>39</v>
       </c>
@@ -1132,7 +1134,7 @@
       </c>
       <c r="C3" s="19"/>
     </row>
-    <row r="4" spans="1:3" ht="23">
+    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>40</v>
       </c>
@@ -1141,7 +1143,7 @@
       </c>
       <c r="C4" s="19"/>
     </row>
-    <row r="5" spans="1:3" ht="23">
+    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>41</v>
       </c>
@@ -1150,7 +1152,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="23">
+    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>43</v>
       </c>
@@ -1162,11 +1164,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1178,9 +1175,9 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" s="16" customFormat="1" ht="23">
+    <row r="1" spans="1:8" s="16" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>45</v>
       </c>
@@ -1204,7 +1201,7 @@
       </c>
       <c r="H1" s="22"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>50</v>
       </c>
@@ -1215,11 +1212,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1227,13 +1219,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>52</v>
       </c>
@@ -1250,7 +1242,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>55</v>
       </c>
@@ -1267,7 +1259,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>55</v>
       </c>
@@ -1284,7 +1276,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>62</v>
       </c>
@@ -1304,10 +1296,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
various fixes leading up to beta release. still need to check data view for token mode
</commit_message>
<xml_diff>
--- a/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
+++ b/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="260" yWindow="460" windowWidth="28540" windowHeight="16220" tabRatio="989" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22680" windowHeight="16220" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
     <sheet name="settings" sheetId="3" r:id="rId2"/>
-    <sheet name="table_specific_translations" sheetId="6" r:id="rId3"/>
-    <sheet name="survey" sheetId="4" r:id="rId4"/>
-    <sheet name="properties" sheetId="5" r:id="rId5"/>
+    <sheet name="survey" sheetId="4" r:id="rId3"/>
+    <sheet name="properties" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>type</t>
   </si>
@@ -178,67 +177,13 @@
   </si>
   <si>
     <t>for_member</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Custom Delivery Form ID</t>
-  </si>
-  <si>
-    <t>Item Pack ID</t>
-  </si>
-  <si>
-    <t>Item Pack Name</t>
-  </si>
-  <si>
-    <t>Item Pack Description</t>
-  </si>
-  <si>
-    <t>Item Pack Ranges</t>
-  </si>
-  <si>
-    <t>Report Version</t>
-  </si>
-  <si>
-    <t>Restrict Overrides</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Status Reason</t>
-  </si>
-  <si>
-    <t>Summary Form ID</t>
-  </si>
-  <si>
-    <t>Date Created</t>
-  </si>
-  <si>
-    <t>Entitlement Generated for Member</t>
-  </si>
-  <si>
-    <t>string_token</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>text.spanish</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -261,15 +206,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,14 +250,8 @@
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -375,26 +307,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -417,11 +334,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -987,164 +899,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1187,7 +945,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>

</xml_diff>

<commit_message>
change authorization definition restrict_overrides->extra_field_entitlements
</commit_message>
<xml_diff>
--- a/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
+++ b/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22680" windowHeight="16220" tabRatio="989" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22680" windowHeight="16220" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>report_version</t>
   </si>
   <si>
-    <t>restrict_overrides</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
@@ -177,6 +174,9 @@
   </si>
   <si>
     <t>for_member</t>
+  </si>
+  <si>
+    <t>extra_field_entitlements</t>
   </si>
 </sst>
 </file>
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -776,7 +776,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -784,7 +784,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -792,7 +792,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -800,7 +800,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -808,7 +808,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -816,7 +816,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -837,27 +837,27 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>19</v>
       </c>
       <c r="C2" s="14"/>
     </row>
     <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="13">
         <v>20170919</v>
@@ -866,28 +866,28 @@
     </row>
     <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="14"/>
     </row>
     <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>25</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -901,7 +901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -909,34 +909,34 @@
   <sheetData>
     <row r="1" spans="1:8" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>29</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>30</v>
       </c>
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
         <v>31</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -957,70 +957,70 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="18" t="s">
         <v>34</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>35</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="C2" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="D2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>38</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>37</v>
-      </c>
       <c r="C3" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="E3" s="19" t="s">
         <v>41</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="C4" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="D4" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>45</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update visit_programs with location information and authorizations with distribution information
</commit_message>
<xml_diff>
--- a/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
+++ b/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/new_redcross_repos/redcross-app-designer/app/config/tables/authorizations/forms/authorizations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarice\red-cross\redcross-app-designer\app\config\tables\authorizations\forms\authorizations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22680" windowHeight="16220" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="22680" windowHeight="16215" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t>type</t>
   </si>
@@ -177,12 +177,18 @@
   </si>
   <si>
     <t>extra_field_entitlements</t>
+  </si>
+  <si>
+    <t>distribution_id</t>
+  </si>
+  <si>
+    <t>distribution_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -251,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -287,40 +293,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -411,6 +394,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -679,19 +665,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="47.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="47.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,7 +685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -707,7 +693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -715,7 +701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -723,7 +709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -731,7 +717,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -739,7 +725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -747,7 +733,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -755,7 +741,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -763,7 +749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -771,7 +757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -779,7 +765,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -787,41 +773,57 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="7" t="s">
+    <row r="13" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="7" t="s">
+    <row r="14" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="8" t="s">
+    <row r="15" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="8" t="s">
+    <row r="16" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -833,63 +835,63 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="14"/>
-    </row>
-    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="10">
         <v>20170919</v>
       </c>
-      <c r="C3" s="14"/>
-    </row>
-    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="14"/>
-    </row>
-    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="14"/>
+      <c r="C6" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -905,13 +907,13 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -920,18 +922,18 @@
       <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="17"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>30</v>
       </c>
@@ -953,73 +955,73 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="19" t="s">
+      <c r="D2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="18" t="s">
+      <c r="D4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove unused fields and add distribution_name to entitlements and deliveries tables
</commit_message>
<xml_diff>
--- a/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
+++ b/app/config/tables/authorizations/forms/authorizations/authorizations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="22680" windowHeight="16215" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="22680" windowHeight="16220" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>type</t>
   </si>
@@ -44,9 +44,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>custom_delivery_form_id</t>
   </si>
   <si>
@@ -62,18 +59,12 @@
     <t>item_pack_ranges</t>
   </si>
   <si>
-    <t>report_version</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
     <t>status_reason</t>
   </si>
   <si>
-    <t>summary_form_id</t>
-  </si>
-  <si>
     <t>date_created</t>
   </si>
   <si>
@@ -105,9 +96,6 @@
   </si>
   <si>
     <t>instance_name</t>
-  </si>
-  <si>
-    <t>data('authorization_name)</t>
   </si>
   <si>
     <t>clause</t>
@@ -665,19 +653,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.375" customWidth="1"/>
-    <col min="2" max="2" width="47.375" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -685,7 +673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -693,55 +681,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -749,76 +737,44 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B11" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B12" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -832,64 +788,67 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="9" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="11"/>
-    </row>
-    <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>19</v>
       </c>
       <c r="B3" s="10">
         <v>20170919</v>
       </c>
       <c r="C3" s="11"/>
     </row>
-    <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="9" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" s="11"/>
-    </row>
-    <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C6" s="11"/>
     </row>
@@ -903,42 +862,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -955,74 +914,74 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="D3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="E3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="16" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="15" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="15" t="s">
+      <c r="B4" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="C4" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="D4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>